<commit_message>
Revert "Merge pull request #51 from nablarch/feature-NAB-8"
This reverts commit eb923c90746405d5bbf5cce304da1ccfec91d547, reversing
changes made to bb4544e55cc87fea634bde57b2cc4395723a3378.
</commit_message>
<xml_diff>
--- a/application_framework/application_framework/libraries/images/mail/images.xlsx
+++ b/application_framework/application_framework/libraries/images/mail/images.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="28035" windowHeight="14580" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="28035" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -25,7 +24,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,19 +43,6 @@
     <font>
       <b/>
       <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="メイリオ"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="メイリオ"/>
@@ -86,17 +72,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -817,711 +797,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="角丸四角形 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2800351" y="857250"/>
-          <a:ext cx="2400300" cy="857250"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" u="sng" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>ステータスを送信済みに変更</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" u="sng" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>メール送信前にステータスを更新する</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>※</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>別トランザクションで実行する</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="角丸四角形 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2800351" y="2143125"/>
-          <a:ext cx="2400300" cy="942975"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" u="sng" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>メール送信を行う</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>メール送信にトランザクションはないため、即送信処理が実行される。</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="直線矢印コネクタ 6"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="4" idx="2"/>
-          <a:endCxn id="5" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4000501" y="1714500"/>
-          <a:ext cx="0" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="フローチャート : 判断 15"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2800350" y="3428999"/>
-          <a:ext cx="2400300" cy="714375"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartDecision">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>送信成功？</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="直線矢印コネクタ 16"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="5" idx="2"/>
-          <a:endCxn id="16" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4000500" y="3086100"/>
-          <a:ext cx="1" cy="342899"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="角丸四角形 19"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5800725" y="3429000"/>
-          <a:ext cx="1800225" cy="752475"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>次のメール送信データへ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>138113</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="直線矢印コネクタ 21"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="16" idx="3"/>
-          <a:endCxn id="20" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5200650" y="3805238"/>
-          <a:ext cx="600075" cy="4761"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="角丸四角形 32"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2800350" y="4543425"/>
-          <a:ext cx="2400300" cy="1028700"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" u="sng" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>ステータスを更新失敗に変更</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" u="sng" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" u="none" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>メール送信時に例外が発生した場合は、ステータスを更新失敗に変更する。</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" u="none" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" u="none" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>※</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" u="none" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>別トランザクションで実行する</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" u="none" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="直線矢印コネクタ 33"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="16" idx="2"/>
-          <a:endCxn id="33" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4000500" y="4190999"/>
-          <a:ext cx="0" cy="352426"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="テキスト ボックス 54"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5200650" y="3600449"/>
-          <a:ext cx="600075" cy="371475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" b="0" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>成功</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="56" name="テキスト ボックス 55"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3943350" y="4171950"/>
-          <a:ext cx="600075" cy="371475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800" b="0" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>失敗</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1816,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1833,28 +1108,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="U21:AA25"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AQ24" sqref="AQ24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="21" spans="21:27" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="AA21" s="3"/>
-    </row>
-    <row r="25" spans="21:27" ht="15" x14ac:dyDescent="0.15">
-      <c r="U25" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>